<commit_message>
EPI Data Entry Page
</commit_message>
<xml_diff>
--- a/VectorSurveillanceDataEntry/IndoorUpdated.xlsx
+++ b/VectorSurveillanceDataEntry/IndoorUpdated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EOL\source\repos\VectorSurveillanceDataEntry\VectorSurveillanceDataEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6BF1C7-DD64-4A51-B05E-C3A0884279E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78D4012-925D-48F4-A35B-A2E21BE12F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,12 +83,6 @@
     <t>Kirto</t>
   </si>
   <si>
-    <t>Narang Urban 5</t>
-  </si>
-  <si>
-    <t>Narang Urban 6</t>
-  </si>
-  <si>
     <t>Lambrey</t>
   </si>
   <si>
@@ -102,6 +96,12 @@
   </si>
   <si>
     <t>Kuthiala Virkan</t>
+  </si>
+  <si>
+    <t>Narang Urban 5</t>
+  </si>
+  <si>
+    <t>Narang Urban 6</t>
   </si>
 </sst>
 </file>
@@ -921,13 +921,13 @@
   <dimension ref="A1:AL23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="38" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -936,10 +936,10 @@
         <v>225</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D1" s="1">
         <v>0</v>
@@ -951,97 +951,97 @@
         <v>0</v>
       </c>
       <c r="G1" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1">
         <v>0</v>
       </c>
       <c r="I1" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1">
         <v>0</v>
       </c>
       <c r="K1" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="L1" s="1">
         <v>0</v>
       </c>
       <c r="M1" s="1">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="N1" s="1">
         <v>0</v>
       </c>
       <c r="O1" s="1">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="P1" s="1">
         <v>0</v>
       </c>
       <c r="Q1" s="1">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="R1" s="1">
         <v>0</v>
       </c>
       <c r="S1" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1">
         <v>0</v>
       </c>
       <c r="U1" s="1">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="V1" s="1">
         <v>0</v>
       </c>
       <c r="W1" s="1">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="X1" s="1">
         <v>0</v>
       </c>
       <c r="Y1" s="1">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="Z1" s="1">
         <v>0</v>
       </c>
       <c r="AA1" s="1">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="AB1" s="1">
         <v>0</v>
       </c>
       <c r="AC1" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="AD1" s="1">
         <v>0</v>
       </c>
       <c r="AE1" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="AF1" s="1">
         <v>0</v>
       </c>
       <c r="AG1" s="1">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AH1" s="1">
         <v>0</v>
       </c>
       <c r="AI1" s="1">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="AJ1" s="1">
         <v>0</v>
       </c>
       <c r="AK1" s="1">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="AL1" s="1">
         <v>0</v>
@@ -1052,10 +1052,10 @@
         <v>226</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -1067,97 +1067,97 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H2" s="1">
         <v>0</v>
       </c>
       <c r="I2" s="1">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>35</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>85</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>96</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>15</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
+        <v>23</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0</v>
+      </c>
+      <c r="U2" s="1">
         <v>10</v>
       </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>24</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>7</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1">
-        <v>13</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1">
-        <v>29</v>
-      </c>
       <c r="V2" s="1">
         <v>0</v>
       </c>
       <c r="W2" s="1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="X2" s="1">
         <v>0</v>
       </c>
       <c r="Y2" s="1">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="Z2" s="1">
         <v>0</v>
       </c>
       <c r="AA2" s="1">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="AB2" s="1">
         <v>0</v>
       </c>
       <c r="AC2" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD2" s="1">
         <v>0</v>
       </c>
       <c r="AE2" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF2" s="1">
         <v>0</v>
       </c>
       <c r="AG2" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AJ2" s="1">
         <v>0</v>
       </c>
       <c r="AK2" s="1">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="AL2" s="1">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -1183,13 +1183,13 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -1213,19 +1213,19 @@
         <v>0</v>
       </c>
       <c r="Q3" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R3" s="1">
         <v>0</v>
       </c>
       <c r="S3" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
       </c>
       <c r="U3" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V3" s="1">
         <v>0</v>
@@ -1261,19 +1261,19 @@
         <v>0</v>
       </c>
       <c r="AG3" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AJ3" s="1">
         <v>0</v>
       </c>
       <c r="AK3" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AL3" s="1">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -1305,13 +1305,13 @@
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
       <c r="K4" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="1">
         <v>0</v>
@@ -1323,19 +1323,19 @@
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
       </c>
       <c r="Q4" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R4" s="1">
         <v>0</v>
       </c>
       <c r="S4" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T4" s="1">
         <v>0</v>
@@ -1353,13 +1353,13 @@
         <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Z4" s="1">
         <v>0</v>
       </c>
       <c r="AA4" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB4" s="1">
         <v>0</v>
@@ -1377,19 +1377,19 @@
         <v>0</v>
       </c>
       <c r="AG4" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH4" s="1">
         <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AJ4" s="1">
         <v>0</v>
       </c>
       <c r="AK4" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AL4" s="1">
         <v>0</v>
@@ -1400,7 +1400,7 @@
         <v>229</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>120</v>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1439,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>0</v>
       </c>
       <c r="S5" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T5" s="1">
         <v>0</v>
@@ -1463,13 +1463,13 @@
         <v>0</v>
       </c>
       <c r="W5" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X5" s="1">
         <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z5" s="1">
         <v>0</v>
@@ -1493,13 +1493,13 @@
         <v>0</v>
       </c>
       <c r="AG5" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AH5" s="1">
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="AJ5" s="1">
         <v>0</v>
@@ -1516,16 +1516,16 @@
         <v>230</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
@@ -1549,13 +1549,13 @@
         <v>0</v>
       </c>
       <c r="M6" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N6" s="1">
         <v>0</v>
       </c>
       <c r="O6" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
@@ -1573,7 +1573,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V6" s="1">
         <v>0</v>
@@ -1591,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="AA6" s="1">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="AB6" s="1">
         <v>0</v>
@@ -1609,13 +1609,13 @@
         <v>0</v>
       </c>
       <c r="AG6" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="1">
         <v>0</v>
       </c>
       <c r="AI6" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AJ6" s="1">
         <v>0</v>
@@ -1653,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
@@ -1671,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
@@ -1683,13 +1683,13 @@
         <v>0</v>
       </c>
       <c r="S7" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="T7" s="1">
         <v>0</v>
       </c>
       <c r="U7" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V7" s="1">
         <v>0</v>
@@ -1701,13 +1701,13 @@
         <v>0</v>
       </c>
       <c r="Y7" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Z7" s="1">
         <v>0</v>
       </c>
       <c r="AA7" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AB7" s="1">
         <v>0</v>
@@ -1725,19 +1725,19 @@
         <v>0</v>
       </c>
       <c r="AG7" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="1">
         <v>0</v>
       </c>
       <c r="AI7" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AJ7" s="1">
         <v>0</v>
       </c>
       <c r="AK7" s="1">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="AL7" s="1">
         <v>0</v>
@@ -1751,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -1763,13 +1763,13 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V8" s="1">
         <v>0</v>
@@ -1817,13 +1817,13 @@
         <v>0</v>
       </c>
       <c r="Y8" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Z8" s="1">
         <v>0</v>
       </c>
       <c r="AA8" s="1">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AB8" s="1">
         <v>0</v>
@@ -1841,19 +1841,19 @@
         <v>0</v>
       </c>
       <c r="AG8" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AH8" s="1">
         <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="AJ8" s="1">
         <v>0</v>
       </c>
       <c r="AK8" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="AL8" s="1">
         <v>0</v>
@@ -1867,7 +1867,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -1903,13 +1903,13 @@
         <v>0</v>
       </c>
       <c r="O9" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P9" s="1">
         <v>0</v>
       </c>
       <c r="Q9" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R9" s="1">
         <v>0</v>
@@ -1939,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="AA9" s="1">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AB9" s="1">
         <v>0</v>
@@ -1957,19 +1957,19 @@
         <v>0</v>
       </c>
       <c r="AG9" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH9" s="1">
         <v>0</v>
       </c>
       <c r="AI9" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AJ9" s="1">
         <v>0</v>
       </c>
       <c r="AK9" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AL9" s="1">
         <v>0</v>
@@ -1980,10 +1980,10 @@
         <v>234</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -1995,19 +1995,19 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
       <c r="I10" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10" s="1">
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R10" s="1">
         <v>0</v>
@@ -2055,7 +2055,7 @@
         <v>0</v>
       </c>
       <c r="AA10" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AB10" s="1">
         <v>0</v>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="AG10" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="1">
         <v>0</v>
@@ -2099,19 +2099,19 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -2123,19 +2123,19 @@
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
       </c>
       <c r="M11" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N11" s="1">
         <v>0</v>
       </c>
       <c r="O11" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="P11" s="1">
         <v>0</v>
@@ -2147,13 +2147,13 @@
         <v>0</v>
       </c>
       <c r="S11" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="T11" s="1">
         <v>0</v>
       </c>
       <c r="U11" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="V11" s="1">
         <v>0</v>
@@ -2165,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Z11" s="1">
         <v>0</v>
@@ -2189,19 +2189,19 @@
         <v>0</v>
       </c>
       <c r="AG11" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="1">
         <v>0</v>
       </c>
       <c r="AI11" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="AJ11" s="1">
         <v>0</v>
       </c>
       <c r="AK11" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AL11" s="1">
         <v>0</v>
@@ -2215,13 +2215,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -2239,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L12" s="1">
         <v>0</v>
@@ -2251,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
@@ -2263,13 +2263,13 @@
         <v>0</v>
       </c>
       <c r="S12" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="T12" s="1">
         <v>0</v>
       </c>
       <c r="U12" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="V12" s="1">
         <v>0</v>
@@ -2299,25 +2299,25 @@
         <v>0</v>
       </c>
       <c r="AE12" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF12" s="1">
         <v>0</v>
       </c>
       <c r="AG12" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="1">
         <v>0</v>
       </c>
       <c r="AI12" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AJ12" s="1">
         <v>0</v>
       </c>
       <c r="AK12" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AL12" s="1">
         <v>0</v>
@@ -2328,10 +2328,10 @@
         <v>237</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
-        <v>112</v>
+        <v>231</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -2343,67 +2343,67 @@
         <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
       <c r="I13" s="1">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
       <c r="K13" s="1">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="L13" s="1">
         <v>0</v>
       </c>
       <c r="M13" s="1">
+        <v>52</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>59</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>12</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
         <v>26</v>
       </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1">
-        <v>27</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>7</v>
-      </c>
-      <c r="R13" s="1">
-        <v>0</v>
-      </c>
-      <c r="S13" s="1">
-        <v>10</v>
-      </c>
       <c r="T13" s="1">
         <v>0</v>
       </c>
       <c r="U13" s="1">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="V13" s="1">
         <v>0</v>
       </c>
       <c r="W13" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="X13" s="1">
         <v>0</v>
       </c>
       <c r="Y13" s="1">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="Z13" s="1">
         <v>0</v>
       </c>
       <c r="AA13" s="1">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="AB13" s="1">
         <v>0</v>
@@ -2415,25 +2415,25 @@
         <v>0</v>
       </c>
       <c r="AE13" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AF13" s="1">
         <v>0</v>
       </c>
       <c r="AG13" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="AH13" s="1">
         <v>0</v>
       </c>
       <c r="AI13" s="1">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="AJ13" s="1">
         <v>0</v>
       </c>
       <c r="AK13" s="1">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="AL13" s="1">
         <v>0</v>
@@ -2444,16 +2444,16 @@
         <v>238</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -2465,25 +2465,25 @@
         <v>0</v>
       </c>
       <c r="I14" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
       </c>
       <c r="K14" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L14" s="1">
         <v>0</v>
       </c>
       <c r="M14" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
       </c>
       <c r="O14" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="P14" s="1">
         <v>0</v>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="S14" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="T14" s="1">
         <v>0</v>
@@ -2507,19 +2507,19 @@
         <v>0</v>
       </c>
       <c r="W14" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="X14" s="1">
         <v>0</v>
       </c>
       <c r="Y14" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Z14" s="1">
         <v>0</v>
       </c>
       <c r="AA14" s="1">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="AB14" s="1">
         <v>0</v>
@@ -2537,19 +2537,19 @@
         <v>0</v>
       </c>
       <c r="AG14" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AH14" s="1">
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="AJ14" s="1">
         <v>0</v>
       </c>
       <c r="AK14" s="1">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="AL14" s="1">
         <v>0</v>
@@ -2563,13 +2563,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F15" s="1">
         <v>0</v>
@@ -2599,19 +2599,19 @@
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
       </c>
       <c r="Q15" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R15" s="1">
         <v>0</v>
       </c>
       <c r="S15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T15" s="1">
         <v>0</v>
@@ -2635,7 +2635,7 @@
         <v>0</v>
       </c>
       <c r="AA15" s="1">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AB15" s="1">
         <v>0</v>
@@ -2653,19 +2653,19 @@
         <v>0</v>
       </c>
       <c r="AG15" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="1">
         <v>0</v>
       </c>
       <c r="AI15" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AJ15" s="1">
         <v>0</v>
       </c>
       <c r="AK15" s="1">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AL15" s="1">
         <v>0</v>
@@ -2679,19 +2679,19 @@
         <v>5</v>
       </c>
       <c r="C16" s="1">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
@@ -2703,19 +2703,19 @@
         <v>0</v>
       </c>
       <c r="K16" s="1">
+        <v>24</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
         <v>26</v>
       </c>
-      <c r="L16" s="1">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>27</v>
-      </c>
       <c r="N16" s="1">
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P16" s="1">
         <v>0</v>
@@ -2727,7 +2727,7 @@
         <v>0</v>
       </c>
       <c r="S16" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T16" s="1">
         <v>0</v>
@@ -2745,13 +2745,13 @@
         <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Z16" s="1">
         <v>0</v>
       </c>
       <c r="AA16" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB16" s="1">
         <v>0</v>
@@ -2769,19 +2769,19 @@
         <v>0</v>
       </c>
       <c r="AG16" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="AH16" s="1">
         <v>0</v>
       </c>
       <c r="AI16" s="1">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AJ16" s="1">
         <v>0</v>
       </c>
       <c r="AK16" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AL16" s="1">
         <v>0</v>
@@ -2795,25 +2795,25 @@
         <v>6</v>
       </c>
       <c r="C17" s="1">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
       <c r="E17" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
       </c>
       <c r="I17" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J17" s="1">
         <v>0</v>
@@ -2831,7 +2831,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P17" s="1">
         <v>0</v>
@@ -2855,19 +2855,19 @@
         <v>0</v>
       </c>
       <c r="W17" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="X17" s="1">
         <v>0</v>
       </c>
       <c r="Y17" s="1">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="Z17" s="1">
         <v>0</v>
       </c>
       <c r="AA17" s="1">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB17" s="1">
         <v>0</v>
@@ -2885,19 +2885,19 @@
         <v>0</v>
       </c>
       <c r="AG17" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH17" s="1">
         <v>0</v>
       </c>
       <c r="AI17" s="1">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AJ17" s="1">
         <v>0</v>
       </c>
       <c r="AK17" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AL17" s="1">
         <v>0</v>
@@ -2911,31 +2911,31 @@
         <v>7</v>
       </c>
       <c r="C18" s="1">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
       </c>
       <c r="I18" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J18" s="1">
         <v>0</v>
       </c>
       <c r="K18" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
@@ -2947,13 +2947,13 @@
         <v>0</v>
       </c>
       <c r="O18" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
       </c>
       <c r="Q18" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R18" s="1">
         <v>0</v>
@@ -2965,7 +2965,7 @@
         <v>0</v>
       </c>
       <c r="U18" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="V18" s="1">
         <v>0</v>
@@ -2977,13 +2977,13 @@
         <v>0</v>
       </c>
       <c r="Y18" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Z18" s="1">
         <v>0</v>
       </c>
       <c r="AA18" s="1">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AB18" s="1">
         <v>0</v>
@@ -3001,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="AG18" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AH18" s="1">
         <v>0</v>
@@ -3027,13 +3027,13 @@
         <v>8</v>
       </c>
       <c r="C19" s="1">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -3045,13 +3045,13 @@
         <v>0</v>
       </c>
       <c r="I19" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
       </c>
       <c r="K19" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
@@ -3069,13 +3069,13 @@
         <v>0</v>
       </c>
       <c r="Q19" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R19" s="1">
         <v>0</v>
       </c>
       <c r="S19" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
@@ -3087,19 +3087,19 @@
         <v>0</v>
       </c>
       <c r="W19" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X19" s="1">
         <v>0</v>
       </c>
       <c r="Y19" s="1">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="Z19" s="1">
         <v>0</v>
       </c>
       <c r="AA19" s="1">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB19" s="1">
         <v>0</v>
@@ -3117,13 +3117,13 @@
         <v>0</v>
       </c>
       <c r="AG19" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AH19" s="1">
         <v>0</v>
       </c>
       <c r="AI19" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AJ19" s="1">
         <v>0</v>
@@ -3149,25 +3149,25 @@
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H20" s="1">
         <v>0</v>
       </c>
       <c r="I20" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
@@ -3191,31 +3191,31 @@
         <v>0</v>
       </c>
       <c r="S20" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>
       </c>
       <c r="U20" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V20" s="1">
         <v>0</v>
       </c>
       <c r="W20" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X20" s="1">
         <v>0</v>
       </c>
       <c r="Y20" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Z20" s="1">
         <v>0</v>
       </c>
       <c r="AA20" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB20" s="1">
         <v>0</v>
@@ -3227,25 +3227,25 @@
         <v>0</v>
       </c>
       <c r="AE20" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AF20" s="1">
         <v>0</v>
       </c>
       <c r="AG20" s="1">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="1">
         <v>0</v>
       </c>
       <c r="AI20" s="1">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="AJ20" s="1">
         <v>0</v>
       </c>
       <c r="AK20" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AL20" s="1">
         <v>0</v>
@@ -3259,37 +3259,37 @@
         <v>10</v>
       </c>
       <c r="C21" s="1">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H21" s="1">
         <v>0</v>
       </c>
       <c r="I21" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
       </c>
       <c r="K21" s="1">
+        <v>26</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
         <v>28</v>
-      </c>
-      <c r="L21" s="1">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1">
-        <v>30</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T21" s="1">
         <v>0</v>
@@ -3325,7 +3325,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="1">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Z21" s="1">
         <v>0</v>
@@ -3343,25 +3343,25 @@
         <v>0</v>
       </c>
       <c r="AE21" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF21" s="1">
         <v>0</v>
       </c>
       <c r="AG21" s="1">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="AH21" s="1">
         <v>0</v>
       </c>
       <c r="AI21" s="1">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AJ21" s="1">
         <v>0</v>
       </c>
       <c r="AK21" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AL21" s="1">
         <v>0</v>
@@ -3375,7 +3375,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="1">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -3393,7 +3393,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J22" s="1">
         <v>0</v>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="AA22" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB22" s="1">
         <v>0</v>
@@ -3465,13 +3465,13 @@
         <v>0</v>
       </c>
       <c r="AG22" s="1">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AH22" s="1">
         <v>0</v>
       </c>
       <c r="AI22" s="1">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AJ22" s="1">
         <v>0</v>
@@ -3491,7 +3491,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -3515,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L23" s="1">
         <v>0</v>
@@ -3527,7 +3527,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -3539,13 +3539,13 @@
         <v>0</v>
       </c>
       <c r="S23" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T23" s="1">
         <v>0</v>
       </c>
       <c r="U23" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V23" s="1">
         <v>0</v>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="AA23" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AB23" s="1">
         <v>0</v>
@@ -3581,13 +3581,13 @@
         <v>0</v>
       </c>
       <c r="AG23" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="AH23" s="1">
         <v>0</v>
       </c>
       <c r="AI23" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AJ23" s="1">
         <v>0</v>

</xml_diff>